<commit_message>
Change column name from "Classifcation" to "Evaluation Category"
</commit_message>
<xml_diff>
--- a/data/TerrestrialAIM_DataAnalysis_Template.xlsx
+++ b/data/TerrestrialAIM_DataAnalysis_Template.xlsx
@@ -3919,9 +3919,6 @@
     <t>Evaluation Stratum</t>
   </si>
   <si>
-    <t>Classification</t>
-  </si>
-  <si>
     <t>GRSG habitat</t>
   </si>
   <si>
@@ -4349,6 +4346,9 @@
   </si>
   <si>
     <t>Proportion Relation</t>
+  </si>
+  <si>
+    <t>Evaluation Category</t>
   </si>
 </sst>
 </file>
@@ -5645,11 +5645,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="118190080"/>
-        <c:axId val="60707328"/>
+        <c:axId val="119566336"/>
+        <c:axId val="58413568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118190080"/>
+        <c:axId val="119566336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5686,7 +5686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60707328"/>
+        <c:crossAx val="58413568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5694,7 +5694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60707328"/>
+        <c:axId val="58413568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5743,7 +5743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118190080"/>
+        <c:crossAx val="119566336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5919,11 +5919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="69719552"/>
-        <c:axId val="60709056"/>
+        <c:axId val="74368512"/>
+        <c:axId val="58415296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69719552"/>
+        <c:axId val="74368512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5960,7 +5960,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60709056"/>
+        <c:crossAx val="58415296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5968,7 +5968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60709056"/>
+        <c:axId val="58415296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6017,7 +6017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69719552"/>
+        <c:crossAx val="74368512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8520,8 +8520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8540,8 +8540,8 @@
     <col min="13" max="13" width="15.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.140625" style="3"/>
     <col min="16" max="16" width="8" style="3" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="27" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -8549,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="92" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C1" s="96" t="s">
         <v>1218</v>
@@ -8573,13 +8573,13 @@
         <v>892</v>
       </c>
       <c r="J1" s="100" t="s">
-        <v>1219</v>
+        <v>1362</v>
       </c>
       <c r="K1" s="100" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="L1" s="93" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="M1" s="28"/>
       <c r="N1" s="29"/>
@@ -8618,7 +8618,7 @@
         <v>893</v>
       </c>
       <c r="J2" s="101" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K2" s="105" t="s">
         <v>890</v>
@@ -8645,7 +8645,7 @@
         <v>885</v>
       </c>
       <c r="C3" s="98" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D3" s="35">
         <v>0</v>
@@ -8654,7 +8654,7 @@
         <v>891</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>891</v>
@@ -8666,7 +8666,7 @@
         <v>893</v>
       </c>
       <c r="J3" s="102" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K3" s="106" t="s">
         <v>888</v>
@@ -8686,7 +8686,7 @@
         <v>885</v>
       </c>
       <c r="C4" s="98" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D4" s="35">
         <v>15</v>
@@ -8695,7 +8695,7 @@
         <v>888</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="G4" s="38" t="s">
         <v>891</v>
@@ -8707,7 +8707,7 @@
         <v>893</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K4" s="106"/>
       <c r="L4" s="40"/>
@@ -8726,7 +8726,7 @@
         <v>885</v>
       </c>
       <c r="C5" s="98" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D5" s="35">
         <v>30</v>
@@ -8735,7 +8735,7 @@
         <v>888</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>891</v>
@@ -8747,7 +8747,7 @@
         <v>893</v>
       </c>
       <c r="J5" s="102" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K5" s="106" t="s">
         <v>890</v>
@@ -8776,7 +8776,7 @@
         <v>891</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>888</v>
@@ -8788,7 +8788,7 @@
         <v>893</v>
       </c>
       <c r="J6" s="103" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K6" s="107" t="s">
         <v>888</v>
@@ -8797,7 +8797,7 @@
         <v>0.1</v>
       </c>
       <c r="Q6" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
@@ -8817,7 +8817,7 @@
         <v>891</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>891</v>
@@ -8829,7 +8829,7 @@
         <v>893</v>
       </c>
       <c r="J7" s="103" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K7" s="107" t="s">
         <v>890</v>
@@ -8855,7 +8855,7 @@
         <v>888</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>891</v>
@@ -8867,7 +8867,7 @@
         <v>893</v>
       </c>
       <c r="J8" s="103" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K8" s="107" t="s">
         <v>888</v>
@@ -8884,7 +8884,7 @@
         <v>884</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="D9" s="11">
         <v>0</v>
@@ -8893,7 +8893,7 @@
         <v>888</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>888</v>
@@ -8905,10 +8905,10 @@
         <v>893</v>
       </c>
       <c r="J9" s="103" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K9" s="107" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="L9" s="15">
         <v>0.75</v>
@@ -8922,7 +8922,7 @@
         <v>884</v>
       </c>
       <c r="C10" s="99" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="D10" s="11">
         <v>20</v>
@@ -8931,7 +8931,7 @@
         <v>891</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>888</v>
@@ -8943,7 +8943,7 @@
         <v>893</v>
       </c>
       <c r="J10" s="103" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K10" s="107" t="s">
         <v>891</v>
@@ -9334,121 +9334,121 @@
         <v>10</v>
       </c>
       <c r="K1" s="32" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="P1" s="32" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Q1" s="32" t="s">
         <v>1291</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>1292</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="S1" s="32" t="s">
+        <v>1294</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>1295</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>1296</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>1297</v>
+      </c>
+      <c r="W1" s="32" t="s">
+        <v>1298</v>
+      </c>
+      <c r="X1" s="32" t="s">
+        <v>1299</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>1300</v>
+      </c>
+      <c r="Z1" s="32" t="s">
+        <v>1301</v>
+      </c>
+      <c r="AA1" s="32" t="s">
+        <v>1302</v>
+      </c>
+      <c r="AB1" s="32" t="s">
+        <v>1303</v>
+      </c>
+      <c r="AC1" s="32" t="s">
+        <v>1304</v>
+      </c>
+      <c r="AD1" s="32" t="s">
+        <v>1305</v>
+      </c>
+      <c r="AE1" s="32" t="s">
+        <v>1306</v>
+      </c>
+      <c r="AF1" s="32" t="s">
+        <v>1307</v>
+      </c>
+      <c r="AG1" s="32" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AH1" s="32" t="s">
+        <v>1309</v>
+      </c>
+      <c r="AI1" s="32" t="s">
+        <v>1310</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
+        <v>1311</v>
+      </c>
+      <c r="AK1" s="32" t="s">
+        <v>1312</v>
+      </c>
+      <c r="AL1" s="32" t="s">
         <v>1293</v>
       </c>
-      <c r="S1" s="32" t="s">
-        <v>1295</v>
-      </c>
-      <c r="T1" s="32" t="s">
-        <v>1296</v>
-      </c>
-      <c r="U1" s="32" t="s">
-        <v>1297</v>
-      </c>
-      <c r="V1" s="32" t="s">
-        <v>1298</v>
-      </c>
-      <c r="W1" s="32" t="s">
-        <v>1299</v>
-      </c>
-      <c r="X1" s="32" t="s">
-        <v>1300</v>
-      </c>
-      <c r="Y1" s="32" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Z1" s="32" t="s">
-        <v>1302</v>
-      </c>
-      <c r="AA1" s="32" t="s">
-        <v>1303</v>
-      </c>
-      <c r="AB1" s="32" t="s">
-        <v>1304</v>
-      </c>
-      <c r="AC1" s="32" t="s">
-        <v>1305</v>
-      </c>
-      <c r="AD1" s="32" t="s">
-        <v>1306</v>
-      </c>
-      <c r="AE1" s="32" t="s">
-        <v>1307</v>
-      </c>
-      <c r="AF1" s="32" t="s">
-        <v>1308</v>
-      </c>
-      <c r="AG1" s="32" t="s">
-        <v>1309</v>
-      </c>
-      <c r="AH1" s="32" t="s">
-        <v>1310</v>
-      </c>
-      <c r="AI1" s="32" t="s">
-        <v>1311</v>
-      </c>
-      <c r="AJ1" s="32" t="s">
-        <v>1312</v>
-      </c>
-      <c r="AK1" s="32" t="s">
+      <c r="AM1" s="32" t="s">
+        <v>1260</v>
+      </c>
+      <c r="AN1" s="32" t="s">
+        <v>1262</v>
+      </c>
+      <c r="AO1" s="32" t="s">
+        <v>1264</v>
+      </c>
+      <c r="AP1" s="32" t="s">
+        <v>1266</v>
+      </c>
+      <c r="AQ1" s="32" t="s">
+        <v>1268</v>
+      </c>
+      <c r="AR1" s="32" t="s">
+        <v>1270</v>
+      </c>
+      <c r="AS1" s="32" t="s">
         <v>1313</v>
       </c>
-      <c r="AL1" s="32" t="s">
-        <v>1294</v>
-      </c>
-      <c r="AM1" s="32" t="s">
-        <v>1261</v>
-      </c>
-      <c r="AN1" s="32" t="s">
-        <v>1263</v>
-      </c>
-      <c r="AO1" s="32" t="s">
-        <v>1265</v>
-      </c>
-      <c r="AP1" s="32" t="s">
-        <v>1267</v>
-      </c>
-      <c r="AQ1" s="32" t="s">
-        <v>1269</v>
-      </c>
-      <c r="AR1" s="32" t="s">
-        <v>1271</v>
-      </c>
-      <c r="AS1" s="32" t="s">
-        <v>1314</v>
-      </c>
       <c r="AT1" s="32" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AU1" s="32" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="AV1" s="32" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AW1" s="32" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AX1" s="32" t="s">
         <v>49</v>
@@ -82961,725 +82961,725 @@
         <v>897</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>1289</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C2" t="s">
         <v>1226</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1291</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1227</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B3" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C3" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B4" t="s">
         <v>1229</v>
       </c>
-      <c r="B4" t="s">
-        <v>1230</v>
-      </c>
       <c r="C4" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B5" t="s">
         <v>1231</v>
       </c>
-      <c r="B5" t="s">
-        <v>1232</v>
-      </c>
       <c r="C5" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B6" t="s">
         <v>1233</v>
       </c>
-      <c r="B6" t="s">
-        <v>1234</v>
-      </c>
       <c r="C6" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B7" t="s">
         <v>1235</v>
       </c>
-      <c r="B7" t="s">
-        <v>1236</v>
-      </c>
       <c r="C7" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B8" t="s">
         <v>1237</v>
       </c>
-      <c r="B8" t="s">
-        <v>1238</v>
-      </c>
       <c r="C8" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B9" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C9" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B10" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C10" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B11" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C11" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B12" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C12" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B13" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C13" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B14" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C14" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B15" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C15" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B16" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C16" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B17" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C17" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B18" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C18" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B19" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C19" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C20" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B21" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B22" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C22" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B23" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C23" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B24" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C24" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B25" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C25" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B26" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C26" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B27" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C27" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B28" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C28" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B29" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C29" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B30" t="s">
         <v>1260</v>
       </c>
-      <c r="B30" t="s">
-        <v>1261</v>
-      </c>
       <c r="C30" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B31" t="s">
         <v>1262</v>
       </c>
-      <c r="B31" t="s">
-        <v>1263</v>
-      </c>
       <c r="C31" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B32" t="s">
         <v>1264</v>
       </c>
-      <c r="B32" t="s">
-        <v>1265</v>
-      </c>
       <c r="C32" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B33" t="s">
         <v>1266</v>
       </c>
-      <c r="B33" t="s">
-        <v>1267</v>
-      </c>
       <c r="C33" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B34" t="s">
         <v>1268</v>
       </c>
-      <c r="B34" t="s">
-        <v>1269</v>
-      </c>
       <c r="C34" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B35" t="s">
         <v>1270</v>
       </c>
-      <c r="B35" t="s">
-        <v>1271</v>
-      </c>
       <c r="C35" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B36" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C36" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B37" t="s">
         <v>1273</v>
       </c>
-      <c r="B37" t="s">
-        <v>1274</v>
-      </c>
       <c r="C37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B38" t="s">
         <v>1275</v>
       </c>
-      <c r="B38" t="s">
-        <v>1276</v>
-      </c>
       <c r="C38" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B39" t="s">
         <v>1277</v>
       </c>
-      <c r="B39" t="s">
-        <v>1278</v>
-      </c>
       <c r="C39" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B40" t="s">
         <v>1279</v>
       </c>
-      <c r="B40" t="s">
-        <v>1280</v>
-      </c>
       <c r="C40" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C41" t="s">
         <v>1281</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1315</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B42" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C42" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B43" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C43" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B44" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C44" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B45" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C45" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B46" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="C46" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B47" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C47" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B48" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="C48" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B49" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C49" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B50" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="C50" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B51" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="C51" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B52" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C52" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B53" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="C53" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B54" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C54" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B55" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C55" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B56" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C56" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B57" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C57" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B58" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C58" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B59" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C59" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B60" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C60" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B61" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C61" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B62" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C62" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B63" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C63" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C64" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B65" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C65" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B66" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C66" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct a few human-readable indicator names
</commit_message>
<xml_diff>
--- a/data/TerrestrialAIM_DataAnalysis_Template.xlsx
+++ b/data/TerrestrialAIM_DataAnalysis_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="-285" windowWidth="24240" windowHeight="8175" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1365" yWindow="-285" windowWidth="24240" windowHeight="8175" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1366">
   <si>
     <t>Management Question</t>
   </si>
@@ -4312,9 +4312,6 @@
     <t>Non-invasive Tree Cover  (%, first hit)</t>
   </si>
   <si>
-    <t>Non-invasive Perennial Forb Cover  (%, first hit)</t>
-  </si>
-  <si>
     <t>Invasive Annual Forb Cover  (%, first hit)</t>
   </si>
   <si>
@@ -4349,6 +4346,18 @@
   </si>
   <si>
     <t>Evaluation Category</t>
+  </si>
+  <si>
+    <t>Bare Soil (%)</t>
+  </si>
+  <si>
+    <t>Invasive Perennial Forb Cover  (%, any hit)</t>
+  </si>
+  <si>
+    <t>Average Sagebrush Height (cm)</t>
+  </si>
+  <si>
+    <t>Invasive Perennial Forb Cover  (%, first hit)</t>
   </si>
 </sst>
 </file>
@@ -5645,11 +5654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="119566336"/>
-        <c:axId val="58413568"/>
+        <c:axId val="155813888"/>
+        <c:axId val="58410112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="119566336"/>
+        <c:axId val="155813888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5686,7 +5695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58413568"/>
+        <c:crossAx val="58410112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5694,7 +5703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58413568"/>
+        <c:axId val="58410112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5743,7 +5752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119566336"/>
+        <c:crossAx val="155813888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5919,11 +5928,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="74368512"/>
-        <c:axId val="58415296"/>
+        <c:axId val="116892160"/>
+        <c:axId val="58412416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74368512"/>
+        <c:axId val="116892160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5960,7 +5969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58415296"/>
+        <c:crossAx val="58412416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5968,7 +5977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58415296"/>
+        <c:axId val="58412416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6017,7 +6026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74368512"/>
+        <c:crossAx val="116892160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8520,7 +8529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8573,13 +8582,13 @@
         <v>892</v>
       </c>
       <c r="J1" s="100" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="K1" s="100" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="L1" s="93" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="M1" s="28"/>
       <c r="N1" s="29"/>
@@ -8797,7 +8806,7 @@
         <v>0.1</v>
       </c>
       <c r="Q6" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
@@ -8908,7 +8917,7 @@
         <v>1221</v>
       </c>
       <c r="K9" s="107" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="L9" s="15">
         <v>0.75</v>
@@ -82945,8 +82954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82972,7 +82981,7 @@
         <v>1225</v>
       </c>
       <c r="B2" t="s">
-        <v>1290</v>
+        <v>1362</v>
       </c>
       <c r="C2" t="s">
         <v>1226</v>
@@ -83159,7 +83168,7 @@
         <v>1248</v>
       </c>
       <c r="B19" t="s">
-        <v>1303</v>
+        <v>1363</v>
       </c>
       <c r="C19" t="s">
         <v>1226</v>
@@ -83302,7 +83311,7 @@
         <v>1263</v>
       </c>
       <c r="B32" t="s">
-        <v>1264</v>
+        <v>1364</v>
       </c>
       <c r="C32" t="s">
         <v>1226</v>
@@ -83588,7 +83597,7 @@
         <v>1331</v>
       </c>
       <c r="B58" t="s">
-        <v>1350</v>
+        <v>1365</v>
       </c>
       <c r="C58" t="s">
         <v>1281</v>
@@ -83599,7 +83608,7 @@
         <v>1332</v>
       </c>
       <c r="B59" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C59" t="s">
         <v>1281</v>
@@ -83610,7 +83619,7 @@
         <v>1333</v>
       </c>
       <c r="B60" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C60" t="s">
         <v>1281</v>
@@ -83621,7 +83630,7 @@
         <v>1334</v>
       </c>
       <c r="B61" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C61" t="s">
         <v>1281</v>
@@ -83632,7 +83641,7 @@
         <v>1335</v>
       </c>
       <c r="B62" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C62" t="s">
         <v>1281</v>
@@ -83643,7 +83652,7 @@
         <v>1336</v>
       </c>
       <c r="B63" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C63" t="s">
         <v>1281</v>
@@ -83654,7 +83663,7 @@
         <v>1337</v>
       </c>
       <c r="B64" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C64" t="s">
         <v>1281</v>
@@ -83665,7 +83674,7 @@
         <v>1338</v>
       </c>
       <c r="B65" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C65" t="s">
         <v>1281</v>
@@ -83676,7 +83685,7 @@
         <v>1339</v>
       </c>
       <c r="B66" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C66" t="s">
         <v>1281</v>

</xml_diff>